<commit_message>
dev: add IotProperty API
</commit_message>
<xml_diff>
--- a/test/data/test-siemens-sheet.xlsx
+++ b/test/data/test-siemens-sheet.xlsx
@@ -77,7 +77,7 @@
     <t>FLOAT</t>
   </si>
   <si>
-    <t>ABCD</t>
+    <t>DCBA</t>
   </si>
   <si>
     <t>DB1.DBD1004</t>
@@ -1521,8 +1521,8 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
dev: enhance rtsp; modbus support utf8
</commit_message>
<xml_diff>
--- a/test/data/test-siemens-sheet.xlsx
+++ b/test/data/test-siemens-sheet.xlsx
@@ -1524,18 +1524,19 @@
   <sheetPr/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F11"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="18.2166666666667" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
     <col min="2" max="2" width="4.325" customWidth="1"/>
     <col min="3" max="3" width="23.05" customWidth="1"/>
     <col min="4" max="4" width="6.64166666666667" customWidth="1"/>
     <col min="5" max="5" width="6.33333333333333" customWidth="1"/>
-    <col min="6" max="7" width="13.8416666666667" customWidth="1"/>
+    <col min="6" max="6" width="8.125" customWidth="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" spans="1:7">

</xml_diff>